<commit_message>
finished renamings in milkrun both modes
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/MilkrunSampleDataAddresses.xlsx
+++ b/pyloghub/sample_data/MilkrunSampleDataAddresses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D4E60C-7515-4214-8C23-6B86BB433857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17ABB28-335F-4213-AAB6-6C2D45920B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2A053323-46B8-4CB9-9383-1A426147D314}"/>
   </bookViews>
@@ -277,21 +277,12 @@
     <t>costsPerStop</t>
   </si>
   <si>
-    <t>costsPerKm</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
     <t>volume</t>
   </si>
   <si>
-    <t>loadingMeter</t>
-  </si>
-  <si>
-    <t>modus</t>
-  </si>
-  <si>
     <t>depot</t>
   </si>
   <si>
@@ -307,10 +298,19 @@
     <t>endTimeWindow</t>
   </si>
   <si>
-    <t>opportunityCosts</t>
-  </si>
-  <si>
-    <t>maxCapacityLoadingMeter</t>
+    <t>maxCapacityPallets</t>
+  </si>
+  <si>
+    <t>costsPerDistanceUnit</t>
+  </si>
+  <si>
+    <t>pallets</t>
+  </si>
+  <si>
+    <t>pickupDelivery</t>
+  </si>
+  <si>
+    <t>externalCosts</t>
   </si>
 </sst>
 </file>
@@ -430,10 +430,10 @@
     <tableColumn id="8" xr3:uid="{F8BD16D8-EDDF-47A3-8209-1EC51557ECF0}" name="maxRouteDuration"/>
     <tableColumn id="9" xr3:uid="{82B674F4-349D-4AB1-8988-F20E24CD50E5}" name="maxCapacityWeight"/>
     <tableColumn id="10" xr3:uid="{811FEE50-E405-4FBA-A583-BE3E0CB5FDBE}" name="maxCapacityVolume"/>
-    <tableColumn id="11" xr3:uid="{EA63B55A-0AC0-4BAF-8286-700941DB0DBF}" name="maxCapacityLoadingMeter"/>
+    <tableColumn id="11" xr3:uid="{EA63B55A-0AC0-4BAF-8286-700941DB0DBF}" name="maxCapacityPallets"/>
     <tableColumn id="12" xr3:uid="{AA62A1E3-ECA9-4DEE-A715-AF26CBC3EFE6}" name="fixedCosts"/>
     <tableColumn id="13" xr3:uid="{5DDBBFDF-CC22-47FD-9B94-DBB9D68EC594}" name="costsPerStop"/>
-    <tableColumn id="14" xr3:uid="{51908A06-03C0-4830-A3F7-95A39A9331EF}" name="costsPerKm"/>
+    <tableColumn id="14" xr3:uid="{51908A06-03C0-4830-A3F7-95A39A9331EF}" name="costsPerDistanceUnit"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -452,14 +452,14 @@
     <tableColumn id="6" xr3:uid="{AAA37768-BA35-4B92-8F31-1951A04E6344}" name="street"/>
     <tableColumn id="7" xr3:uid="{6AA94278-B185-41C6-B426-99516A6C894D}" name="weight"/>
     <tableColumn id="8" xr3:uid="{BA7651A9-558D-44E6-B84C-1E9E2D72D9C0}" name="volume"/>
-    <tableColumn id="9" xr3:uid="{56808CC6-FBD4-4393-AF34-8FF24B2148A4}" name="loadingMeter"/>
-    <tableColumn id="10" xr3:uid="{E54C3E40-13C9-4162-B2F1-EAFD2DED677E}" name="modus"/>
+    <tableColumn id="9" xr3:uid="{56808CC6-FBD4-4393-AF34-8FF24B2148A4}" name="pallets"/>
+    <tableColumn id="10" xr3:uid="{E54C3E40-13C9-4162-B2F1-EAFD2DED677E}" name="pickupDelivery"/>
     <tableColumn id="11" xr3:uid="{7DF3A7F7-6CF6-45B6-A60A-7539E7C7C1B5}" name="depot"/>
     <tableColumn id="12" xr3:uid="{9CDC32BA-48FB-4C4E-A683-A421F4AAFCBD}" name="vehicleType"/>
     <tableColumn id="13" xr3:uid="{060F4538-B9D1-446B-BE26-ABA52785305B}" name="serviceTime"/>
     <tableColumn id="14" xr3:uid="{8DE0BB8A-AB58-4605-BB4A-EB56DE22EAC6}" name="startTimeWindow" dataDxfId="1"/>
     <tableColumn id="15" xr3:uid="{91F24563-3755-49CB-B895-7E67C14BBB88}" name="endTimeWindow" dataDxfId="0"/>
-    <tableColumn id="16" xr3:uid="{393FA7FC-6C14-4B7B-AFE0-96E0FD235948}" name="opportunityCosts"/>
+    <tableColumn id="16" xr3:uid="{393FA7FC-6C14-4B7B-AFE0-96E0FD235948}" name="externalCosts"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -936,7 +936,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +976,7 @@
         <v>76</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>77</v>
@@ -985,7 +985,7 @@
         <v>78</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,34 +1098,34 @@
         <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>